<commit_message>
Flor Extraction Project: - Implemented basic rule information searching, filtering and organizing
</commit_message>
<xml_diff>
--- a/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
+++ b/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Object_Creation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Flow_Extraction\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18191E24-BEEB-488B-A188-21DDB45E2E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA152C5-CDB9-41CF-9FE9-65F6C92E6587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
@@ -25,39 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Object Name</t>
   </si>
   <si>
-    <t>Object IP</t>
-  </si>
-  <si>
-    <t>Object Groups</t>
-  </si>
-  <si>
-    <t>Local_User</t>
-  </si>
-  <si>
-    <t>Host_12.0.0.1</t>
-  </si>
-  <si>
-    <t>12.0.0.1</t>
-  </si>
-  <si>
-    <t>Host_12.0.0.3</t>
-  </si>
-  <si>
-    <t>12.0.0.3</t>
-  </si>
-  <si>
-    <t>Net_15.0.0.0</t>
-  </si>
-  <si>
-    <t>15.0.0.0/24</t>
-  </si>
-  <si>
-    <t>Remote_User</t>
+    <t>Host_10.0.0.1</t>
   </si>
 </sst>
 </file>
@@ -445,70 +418,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858A042F-E78E-42AB-85EA-A4FEB9F441DE}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="7" max="7" width="27.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="1" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Flow Extraction Project: - Implemented fetching and classifying of access rules' full details - Improved user messages and handling errors
</commit_message>
<xml_diff>
--- a/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
+++ b/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Flow_Extraction\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA152C5-CDB9-41CF-9FE9-65F6C92E6587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E032E70-C69E-48EA-9BE1-B9E6D1671EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
@@ -25,12 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Object Name</t>
   </si>
   <si>
     <t>Host_10.0.0.1</t>
+  </si>
+  <si>
+    <t>Host_10.0.0.2</t>
+  </si>
+  <si>
+    <t>Host_10.0.0.3</t>
+  </si>
+  <si>
+    <t>Host_10.0.0.4</t>
   </si>
 </sst>
 </file>
@@ -421,7 +430,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,13 +451,19 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Flow Extraction Project: - Flows exported to excel file completed
</commit_message>
<xml_diff>
--- a/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
+++ b/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Flow_Extraction\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E032E70-C69E-48EA-9BE1-B9E6D1671EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721386ED-F2F4-4B9D-8E15-47EEEC4C3EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
@@ -30,10 +30,10 @@
     <t>Object Name</t>
   </si>
   <si>
-    <t>Host_10.0.0.1</t>
+    <t>Host_10.0.0.2</t>
   </si>
   <si>
-    <t>Host_10.0.0.2</t>
+    <t>Host_10.0.0.1</t>
   </si>
   <si>
     <t>Host_10.0.0.3</t>
@@ -430,7 +430,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A12" sqref="A6:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,12 +447,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Flow Extraction Project: - Updated README
</commit_message>
<xml_diff>
--- a/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
+++ b/Checkpoint_Flow_Extraction/config/Flow_Extraction-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Flow_Extraction\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721386ED-F2F4-4B9D-8E15-47EEEC4C3EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917EBF9C-F98E-404E-A2ED-3479B3EAB92C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
@@ -25,21 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Object Name</t>
   </si>
   <si>
-    <t>Host_10.0.0.2</t>
-  </si>
-  <si>
-    <t>Host_10.0.0.1</t>
-  </si>
-  <si>
-    <t>Host_10.0.0.3</t>
-  </si>
-  <si>
-    <t>Host_10.0.0.4</t>
+    <t>Net_10.1.0.0_24</t>
   </si>
 </sst>
 </file>
@@ -430,7 +421,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A6:XFD12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,23 +438,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>